<commit_message>
docs(taskplan): update task management for sigin up, sign in
</commit_message>
<xml_diff>
--- a/docs/Task Management.xlsx
+++ b/docs/Task Management.xlsx
@@ -1,34 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repo-Personal-Task-Management-App\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1096C695-9D7F-4704-B4D0-140D17DE08DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <bookViews>
-    <workbookView xWindow="735" yWindow="735" windowWidth="17280" windowHeight="9983" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
   </bookViews>
   <sheets>
-    <sheet name="Task List" sheetId="1" r:id="rId1"/>
+    <sheet name="Task List" sheetId="1" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="25">
   <si>
     <t>Link rept</t>
   </si>
   <si>
     <r>
       <rPr>
-        <b/>
-        <u/>
+        <b val="1"/>
+        <u val="single"/>
         <sz val="12"/>
         <color indexed="8"/>
         <rFont val="Times New Roman"/>
@@ -109,26 +100,37 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="d/m/yy"/>
-    <numFmt numFmtId="165" formatCode="d/m/yyyy"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="3">
+    <numFmt numFmtId="0" formatCode="General"/>
+    <numFmt numFmtId="59" formatCode="d/m/yy"/>
+    <numFmt numFmtId="60" formatCode="d/m/yyyy"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
     </font>
     <font>
-      <b/>
+      <sz val="12"/>
+      <color indexed="8"/>
+      <name val="Helvetica Neue"/>
+    </font>
+    <font>
+      <sz val="15"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b val="1"/>
       <sz val="12"/>
       <color indexed="8"/>
       <name val="Times New Roman"/>
     </font>
     <font>
-      <b/>
-      <u/>
+      <b val="1"/>
+      <u val="single"/>
       <sz val="12"/>
       <color indexed="8"/>
       <name val="Times New Roman"/>
@@ -139,12 +141,18 @@
       <name val="Times New Roman"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+        <bgColor auto="1"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -157,55 +165,52 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+  <cellXfs count="9">
+    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="59" fontId="5" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="60" fontId="5" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -215,85 +220,24 @@
   <tableStyles count="0"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFFF0000"/>
-      <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFA5A5A5"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
+      <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ffffffff"/>
+      <rgbColor rgb="ffff0000"/>
+      <rgbColor rgb="ff00ff00"/>
+      <rgbColor rgb="ff0000ff"/>
+      <rgbColor rgb="ffffff00"/>
+      <rgbColor rgb="ffff00ff"/>
+      <rgbColor rgb="ff00ffff"/>
+      <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ffffffff"/>
+      <rgbColor rgb="ffa5a5a5"/>
     </indexedColors>
   </colors>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Blank">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Blank">
   <a:themeElements>
     <a:clrScheme name="Blank">
       <a:dk1>
@@ -303,10 +247,10 @@
         <a:srgbClr val="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="5E5E5E"/>
+        <a:srgbClr val="A7A7A7"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="D5D5D5"/>
+        <a:srgbClr val="535353"/>
       </a:lt2>
       <a:accent1>
         <a:srgbClr val="00A2FF"/>
@@ -483,46 +427,49 @@
     <a:spDef>
       <a:spPr>
         <a:solidFill>
-          <a:srgbClr val="000000"/>
+          <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
-        <a:ln w="12700" cap="flat">
-          <a:noFill/>
-          <a:miter lim="400000"/>
+        <a:ln w="25400" cap="flat">
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
-        <a:defPPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="584200" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
-          <a:lnSpc>
-            <a:spcPct val="100000"/>
-          </a:lnSpc>
-          <a:spcBef>
-            <a:spcPts val="0"/>
-          </a:spcBef>
-          <a:spcAft>
-            <a:spcPts val="0"/>
-          </a:spcAft>
-          <a:buClrTx/>
-          <a:buSzTx/>
-          <a:buFontTx/>
-          <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1200" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:solidFill>
-              <a:srgbClr val="FFFFFF"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:uFillTx/>
-            <a:latin typeface="Helvetica Neue Medium"/>
-            <a:ea typeface="Helvetica Neue Medium"/>
-            <a:cs typeface="Helvetica Neue Medium"/>
-            <a:sym typeface="Helvetica Neue Medium"/>
+        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -539,7 +486,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -564,7 +511,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -589,7 +536,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -614,7 +561,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -639,7 +586,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -664,7 +611,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -689,7 +636,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -714,7 +661,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -739,7 +686,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -752,32 +699,26 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
     <a:lnDef>
       <a:spPr>
         <a:noFill/>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
-            <a:srgbClr val="000000"/>
+            <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="400000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -795,7 +736,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -820,7 +761,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -845,7 +786,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -870,7 +811,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -895,7 +836,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -920,7 +861,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -945,7 +886,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -970,7 +911,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -995,7 +936,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1020,7 +961,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1033,15 +974,9 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -1055,25 +990,25 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
-        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="457200" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
-          <a:lnSpc>
-            <a:spcPct val="100000"/>
-          </a:lnSpc>
-          <a:spcBef>
-            <a:spcPts val="0"/>
-          </a:spcBef>
-          <a:spcAft>
-            <a:spcPts val="0"/>
-          </a:spcAft>
-          <a:buClrTx/>
-          <a:buSzTx/>
-          <a:buFontTx/>
-          <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1102,7 +1037,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1127,7 +1062,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1152,7 +1087,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1177,7 +1112,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1202,7 +1137,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1227,7 +1162,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1252,7 +1187,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1277,7 +1212,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1302,7 +1237,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1315,340 +1250,338 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
-    </sheetView>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.6640625" defaultRowHeight="19.899999999999999" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="16.6667" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="28.3984375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="14.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="14.19921875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="12.1328125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="12.59765625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="28.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="14.6719" style="1" customWidth="1"/>
+    <col min="3" max="3" width="14.1719" style="1" customWidth="1"/>
+    <col min="4" max="4" width="12.1719" style="1" customWidth="1"/>
+    <col min="5" max="5" width="12.6719" style="1" customWidth="1"/>
     <col min="6" max="6" width="11" style="1" customWidth="1"/>
-    <col min="7" max="7" width="16.6640625" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="16.6640625" style="1"/>
+    <col min="7" max="16384" width="16.6719" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="16.8" customHeight="1">
-      <c r="A1" s="2" t="s">
+    <row r="1" ht="16.8" customHeight="1">
+      <c r="A1" t="s" s="2">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" t="s" s="2">
         <v>1</v>
       </c>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-    </row>
-    <row r="2" spans="1:6" ht="31.8" customHeight="1">
-      <c r="A2" s="2" t="s">
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+    </row>
+    <row r="2" ht="31.8" customHeight="1">
+      <c r="A2" t="s" s="2">
         <v>2</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" t="s" s="2">
         <v>3</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" t="s" s="2">
         <v>4</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" t="s" s="2">
         <v>5</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" t="s" s="2">
         <v>6</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" t="s" s="2">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="16.8" customHeight="1">
-      <c r="A3" s="3" t="s">
+    <row r="3" ht="16.8" customHeight="1">
+      <c r="A3" t="s" s="4">
         <v>8</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" t="s" s="4">
         <v>9</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="5">
         <v>1</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="6">
         <v>45821</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="6">
         <v>45824</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="5">
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="16.8" customHeight="1">
-      <c r="A4" s="3" t="s">
+    <row r="4" ht="16.8" customHeight="1">
+      <c r="A4" t="s" s="4">
         <v>10</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" t="s" s="4">
         <v>9</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="5">
         <v>1</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="6">
         <v>45821</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="6">
         <v>45824</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="5">
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="16.8" customHeight="1">
-      <c r="A5" s="3" t="s">
+    <row r="5" ht="16.8" customHeight="1">
+      <c r="A5" t="s" s="4">
         <v>11</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" t="s" s="4">
         <v>9</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="5">
         <v>3</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="6">
         <v>45824</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="7">
         <v>45826</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="5">
         <v>70</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="16.8" customHeight="1">
-      <c r="A6" s="3" t="s">
+    <row r="6" ht="16.8" customHeight="1">
+      <c r="A6" t="s" s="4">
         <v>12</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" t="s" s="4">
         <v>9</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="5">
         <v>2</v>
       </c>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="4">
+      <c r="D6" s="7">
+        <v>45827</v>
+      </c>
+      <c r="E6" s="7">
+        <v>45831</v>
+      </c>
+      <c r="F6" s="5">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="16.8" customHeight="1">
-      <c r="A7" s="3" t="s">
+    <row r="7" ht="16.8" customHeight="1">
+      <c r="A7" t="s" s="4">
         <v>13</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" t="s" s="4">
         <v>9</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="5">
         <v>2</v>
       </c>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="4">
+      <c r="D7" s="7">
+        <v>45827</v>
+      </c>
+      <c r="E7" s="7">
+        <v>45831</v>
+      </c>
+      <c r="F7" s="5">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="16.8" customHeight="1">
-      <c r="A8" s="3" t="s">
+    <row r="8" ht="16.8" customHeight="1">
+      <c r="A8" t="s" s="4">
         <v>14</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" t="s" s="4">
         <v>9</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="5">
         <v>3</v>
       </c>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="4">
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="5">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="16.8" customHeight="1">
-      <c r="A9" s="3" t="s">
+    <row r="9" ht="16.8" customHeight="1">
+      <c r="A9" t="s" s="4">
         <v>15</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" t="s" s="4">
         <v>9</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9" s="5">
         <v>2</v>
       </c>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="4">
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="5">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="16.8" customHeight="1">
-      <c r="A10" s="3" t="s">
+    <row r="10" ht="16.8" customHeight="1">
+      <c r="A10" t="s" s="4">
         <v>16</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" t="s" s="4">
         <v>9</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10" s="5">
         <v>2</v>
       </c>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="4">
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="5">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="16.8" customHeight="1">
-      <c r="A11" s="3" t="s">
+    <row r="11" ht="16.8" customHeight="1">
+      <c r="A11" t="s" s="4">
         <v>17</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" t="s" s="4">
         <v>9</v>
       </c>
-      <c r="C11" s="4">
+      <c r="C11" s="5">
         <v>2</v>
       </c>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="4">
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="5">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="16.8" customHeight="1">
-      <c r="A12" s="3" t="s">
+    <row r="12" ht="16.8" customHeight="1">
+      <c r="A12" t="s" s="4">
         <v>18</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" t="s" s="4">
         <v>9</v>
       </c>
-      <c r="C12" s="4">
+      <c r="C12" s="5">
         <v>3</v>
       </c>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="4">
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="5">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="16.8" customHeight="1">
-      <c r="A13" s="3" t="s">
+    <row r="13" ht="16.8" customHeight="1">
+      <c r="A13" t="s" s="4">
         <v>19</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" t="s" s="4">
         <v>9</v>
       </c>
-      <c r="C13" s="4">
+      <c r="C13" s="5">
         <v>2</v>
       </c>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="4">
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="5">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="16.8" customHeight="1">
-      <c r="A14" s="3" t="s">
+    <row r="14" ht="16.8" customHeight="1">
+      <c r="A14" t="s" s="4">
         <v>20</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" t="s" s="4">
         <v>9</v>
       </c>
-      <c r="C14" s="4">
+      <c r="C14" s="5">
         <v>2</v>
       </c>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="4">
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="5">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="16.8" customHeight="1">
-      <c r="A15" s="3" t="s">
+    <row r="15" ht="16.8" customHeight="1">
+      <c r="A15" t="s" s="4">
         <v>21</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" t="s" s="4">
         <v>9</v>
       </c>
-      <c r="C15" s="4">
+      <c r="C15" s="5">
         <v>3</v>
       </c>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="4">
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="5">
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="16.8" customHeight="1">
-      <c r="A16" s="3" t="s">
+    <row r="16" ht="16.8" customHeight="1">
+      <c r="A16" t="s" s="4">
         <v>22</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" t="s" s="4">
         <v>9</v>
       </c>
-      <c r="C16" s="4">
+      <c r="C16" s="5">
         <v>2</v>
       </c>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="4">
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="5">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="16.8" customHeight="1">
-      <c r="A17" s="3" t="s">
+    <row r="17" ht="16.8" customHeight="1">
+      <c r="A17" t="s" s="4">
         <v>23</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" t="s" s="4">
         <v>9</v>
       </c>
-      <c r="C17" s="4">
+      <c r="C17" s="5">
         <v>2</v>
       </c>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="4">
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="5">
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="16.8" customHeight="1">
-      <c r="A18" s="3" t="s">
+    <row r="18" ht="16.8" customHeight="1">
+      <c r="A18" t="s" s="4">
         <v>24</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" t="s" s="4">
         <v>9</v>
       </c>
-      <c r="C18" s="4">
+      <c r="C18" s="5">
         <v>2</v>
       </c>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="4">
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="5">
         <v>0</v>
       </c>
     </row>
@@ -1657,10 +1590,10 @@
     <mergeCell ref="B1:F1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B1" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B1" r:id="rId1" location="" tooltip="" display="https://github.com/buitiendat79/Repo-Personal-Task-Management-App"/>
   </hyperlinks>
-  <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.27777800000000002" footer="0.27777800000000002"/>
-  <pageSetup scale="72" orientation="portrait"/>
+  <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="72" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>

</xml_diff>